<commit_message>
Added framework for excel writing
</commit_message>
<xml_diff>
--- a/Schedule-2019-09-24.xlsx
+++ b/Schedule-2019-09-24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mvandewille/Box/ISU/ENGCF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mvandewille/Documents/engcf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EBE46E-C945-C949-8583-E03906D981E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1704BF47-3C0D-154B-8150-D98BF76FCD90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4180,8 +4180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="160" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="117" workbookViewId="0">
+      <selection activeCell="I139" sqref="I139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4774,6 +4774,9 @@
       <c r="B17" t="s">
         <v>42</v>
       </c>
+      <c r="C17">
+        <v>490227758</v>
+      </c>
       <c r="D17" t="s">
         <v>43</v>
       </c>
@@ -5865,6 +5868,9 @@
       <c r="B49" t="s">
         <v>76</v>
       </c>
+      <c r="C49">
+        <v>490227758</v>
+      </c>
       <c r="D49" t="s">
         <v>34</v>
       </c>
@@ -9182,7 +9188,7 @@
         <v>140</v>
       </c>
       <c r="C146">
-        <v>490227758</v>
+        <v>363438107</v>
       </c>
       <c r="D146" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Modified fileUpload.html to do both functions, upload and ID scanning. IDScanner and IDScanner2 no longer within runtime path
</commit_message>
<xml_diff>
--- a/Schedule-2019-09-24.xlsx
+++ b/Schedule-2019-09-24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mvandewille/Documents/engcf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1704BF47-3C0D-154B-8150-D98BF76FCD90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A3D91D-5DAA-0A42-83D6-632A1B900367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hourly - Career Fair" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -4180,8 +4182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="117" workbookViewId="0">
-      <selection activeCell="I139" sqref="I139"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4255,9 +4257,6 @@
       <c r="B2" t="s">
         <v>140</v>
       </c>
-      <c r="C2">
-        <v>490227758</v>
-      </c>
       <c r="D2" t="s">
         <v>56</v>
       </c>
@@ -4292,9 +4291,6 @@
       <c r="B3" t="s">
         <v>140</v>
       </c>
-      <c r="C3">
-        <v>490227758</v>
-      </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
@@ -4329,6 +4325,9 @@
       <c r="B4" t="s">
         <v>120</v>
       </c>
+      <c r="C4">
+        <v>490227758</v>
+      </c>
       <c r="D4" t="s">
         <v>56</v>
       </c>
@@ -4499,9 +4498,6 @@
       <c r="B9" t="s">
         <v>140</v>
       </c>
-      <c r="C9">
-        <v>490227758</v>
-      </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
@@ -5151,6 +5147,9 @@
       <c r="B28" t="s">
         <v>109</v>
       </c>
+      <c r="C28">
+        <v>490227758</v>
+      </c>
       <c r="D28" t="s">
         <v>43</v>
       </c>
@@ -5627,9 +5626,6 @@
       <c r="B42" t="s">
         <v>140</v>
       </c>
-      <c r="C42">
-        <v>490227758</v>
-      </c>
       <c r="D42" t="s">
         <v>8</v>
       </c>
@@ -5868,9 +5864,6 @@
       <c r="B49" t="s">
         <v>76</v>
       </c>
-      <c r="C49">
-        <v>490227758</v>
-      </c>
       <c r="D49" t="s">
         <v>34</v>
       </c>
@@ -6687,9 +6680,6 @@
       <c r="B73" t="s">
         <v>140</v>
       </c>
-      <c r="C73">
-        <v>490227758</v>
-      </c>
       <c r="D73" t="s">
         <v>22</v>
       </c>
@@ -7200,9 +7190,6 @@
       <c r="B88" t="s">
         <v>140</v>
       </c>
-      <c r="C88">
-        <v>490227758</v>
-      </c>
       <c r="D88" t="s">
         <v>36</v>
       </c>
@@ -8257,9 +8244,6 @@
       <c r="B119" t="s">
         <v>140</v>
       </c>
-      <c r="C119">
-        <v>490227758</v>
-      </c>
       <c r="D119" t="s">
         <v>54</v>
       </c>
@@ -8328,9 +8312,6 @@
       <c r="B121" t="s">
         <v>140</v>
       </c>
-      <c r="C121">
-        <v>490227758</v>
-      </c>
       <c r="D121" t="s">
         <v>25</v>
       </c>
@@ -8943,9 +8924,6 @@
       <c r="B139" t="s">
         <v>140</v>
       </c>
-      <c r="C139">
-        <v>490227758</v>
-      </c>
       <c r="D139" t="s">
         <v>16</v>
       </c>
@@ -9014,9 +8992,6 @@
       <c r="B141" t="s">
         <v>64</v>
       </c>
-      <c r="C141">
-        <v>281501244</v>
-      </c>
       <c r="D141" t="s">
         <v>50</v>
       </c>
@@ -9187,9 +9162,6 @@
       <c r="B146" t="s">
         <v>140</v>
       </c>
-      <c r="C146">
-        <v>363438107</v>
-      </c>
       <c r="D146" t="s">
         <v>50</v>
       </c>
@@ -9394,9 +9366,6 @@
       <c r="B152" t="s">
         <v>140</v>
       </c>
-      <c r="C152">
-        <v>490227758</v>
-      </c>
       <c r="D152" t="s">
         <v>67</v>
       </c>
@@ -9407,10 +9376,10 @@
         <v>138</v>
       </c>
       <c r="G152" s="6">
-        <v>43732.791666666664</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="H152" s="6">
-        <v>43732.833333333336</v>
+        <v>0.875</v>
       </c>
       <c r="J152">
         <v>1</v>

</xml_diff>

<commit_message>
Working model of ID swiper writes to excel doc when exported
</commit_message>
<xml_diff>
--- a/Schedule-2019-09-24.xlsx
+++ b/Schedule-2019-09-24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mvandewille/Documents/engcf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepo\engcf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBB1B39-8F08-4348-8873-7BA0C87FE209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEA6904-50E8-4627-A0A5-B75C02885A7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hourly - Career Fair" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="142">
   <si>
     <t>Employee ID</t>
   </si>
@@ -454,6 +454,9 @@
   </si>
   <si>
     <t>Max Van de Wille</t>
+  </si>
+  <si>
+    <t>Katharine Browning</t>
   </si>
 </sst>
 </file>
@@ -816,7 +819,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="3" width="18" customWidth="1"/>
@@ -824,7 +827,7 @@
     <col min="5" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:702" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1544,7 +1547,7 @@
       <c r="ZY1" s="2"/>
       <c r="ZZ1" s="2"/>
     </row>
-    <row r="2" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -1564,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -1584,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:702" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:702" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>14</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -1658,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -1698,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:702" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -1715,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -1735,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>21</v>
       </c>
@@ -1755,7 +1758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>23</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:702" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>16</v>
       </c>
@@ -1792,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -1812,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>26</v>
       </c>
@@ -1832,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>28</v>
       </c>
@@ -1852,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -1872,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>30</v>
       </c>
@@ -1892,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>32</v>
       </c>
@@ -1932,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>33</v>
       </c>
@@ -1952,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>35</v>
       </c>
@@ -1972,7 +1975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>36</v>
       </c>
@@ -1989,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>37</v>
       </c>
@@ -2006,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>38</v>
       </c>
@@ -2026,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>39</v>
       </c>
@@ -2046,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>41</v>
       </c>
@@ -2066,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>42</v>
       </c>
@@ -2086,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>40</v>
       </c>
@@ -2103,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>44</v>
       </c>
@@ -2123,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>22</v>
       </c>
@@ -2140,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>45</v>
       </c>
@@ -2160,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>14</v>
       </c>
@@ -2177,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>46</v>
       </c>
@@ -2197,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>47</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>49</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>51</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>40</v>
       </c>
@@ -2274,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>52</v>
       </c>
@@ -2294,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>53</v>
       </c>
@@ -2314,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>13</v>
       </c>
@@ -2331,7 +2334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>55</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>57</v>
       </c>
@@ -2371,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>14</v>
       </c>
@@ -2388,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>58</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>43</v>
       </c>
@@ -2425,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>40</v>
       </c>
@@ -2442,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>59</v>
       </c>
@@ -2462,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>60</v>
       </c>
@@ -2482,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>61</v>
       </c>
@@ -2502,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>62</v>
       </c>
@@ -2522,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>63</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>64</v>
       </c>
@@ -2562,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>65</v>
       </c>
@@ -2582,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>66</v>
       </c>
@@ -2602,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>67</v>
       </c>
@@ -2619,7 +2622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>68</v>
       </c>
@@ -2639,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>10</v>
       </c>
@@ -2656,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>69</v>
       </c>
@@ -2676,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>11</v>
       </c>
@@ -2693,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>70</v>
       </c>
@@ -2713,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>10</v>
       </c>
@@ -2730,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>71</v>
       </c>
@@ -2750,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>43</v>
       </c>
@@ -2767,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>72</v>
       </c>
@@ -2787,7 +2790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>73</v>
       </c>
@@ -2807,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>74</v>
       </c>
@@ -2827,7 +2830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>14</v>
       </c>
@@ -2844,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>75</v>
       </c>
@@ -2864,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>76</v>
       </c>
@@ -2884,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>77</v>
       </c>
@@ -2904,7 +2907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>78</v>
       </c>
@@ -2924,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>79</v>
       </c>
@@ -2944,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>48</v>
       </c>
@@ -2961,7 +2964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>80</v>
       </c>
@@ -2981,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>81</v>
       </c>
@@ -3001,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>82</v>
       </c>
@@ -3021,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>83</v>
       </c>
@@ -3041,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>84</v>
       </c>
@@ -3061,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>85</v>
       </c>
@@ -3081,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>86</v>
       </c>
@@ -3101,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>87</v>
       </c>
@@ -3121,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>50</v>
       </c>
@@ -3138,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>88</v>
       </c>
@@ -3158,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>89</v>
       </c>
@@ -3178,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>90</v>
       </c>
@@ -3198,7 +3201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>91</v>
       </c>
@@ -3218,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>92</v>
       </c>
@@ -3238,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
         <v>14</v>
       </c>
@@ -3255,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>93</v>
       </c>
@@ -3275,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
         <v>14</v>
       </c>
@@ -3292,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>94</v>
       </c>
@@ -3312,7 +3315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>95</v>
       </c>
@@ -3332,7 +3335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
         <v>11</v>
       </c>
@@ -3349,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>96</v>
       </c>
@@ -3369,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
         <v>54</v>
       </c>
@@ -3386,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>97</v>
       </c>
@@ -3406,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
         <v>54</v>
       </c>
@@ -3423,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>98</v>
       </c>
@@ -3443,7 +3446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>99</v>
       </c>
@@ -3463,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>100</v>
       </c>
@@ -3483,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>101</v>
       </c>
@@ -3503,7 +3506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>102</v>
       </c>
@@ -3523,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C105" t="s">
         <v>27</v>
       </c>
@@ -3540,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>103</v>
       </c>
@@ -3560,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>104</v>
       </c>
@@ -3580,7 +3583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C108" t="s">
         <v>37</v>
       </c>
@@ -3597,7 +3600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>105</v>
       </c>
@@ -3617,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C110" t="s">
         <v>22</v>
       </c>
@@ -3634,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C111" t="s">
         <v>36</v>
       </c>
@@ -3651,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C112" t="s">
         <v>54</v>
       </c>
@@ -3668,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>106</v>
       </c>
@@ -3688,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>107</v>
       </c>
@@ -3708,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>108</v>
       </c>
@@ -3728,7 +3731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>109</v>
       </c>
@@ -3748,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>110</v>
       </c>
@@ -3768,7 +3771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>111</v>
       </c>
@@ -3788,7 +3791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>112</v>
       </c>
@@ -3808,7 +3811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>113</v>
       </c>
@@ -3828,7 +3831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
         <v>36</v>
       </c>
@@ -3845,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
         <v>67</v>
       </c>
@@ -3862,7 +3865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>114</v>
       </c>
@@ -3882,7 +3885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>115</v>
       </c>
@@ -3902,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>116</v>
       </c>
@@ -3922,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>118</v>
       </c>
@@ -3942,7 +3945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C127" t="s">
         <v>34</v>
       </c>
@@ -3959,7 +3962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>119</v>
       </c>
@@ -3979,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>120</v>
       </c>
@@ -3999,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>121</v>
       </c>
@@ -4019,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>122</v>
       </c>
@@ -4039,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C132" t="s">
         <v>11</v>
       </c>
@@ -4056,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>123</v>
       </c>
@@ -4076,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>124</v>
       </c>
@@ -4096,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
         <v>36</v>
       </c>
@@ -4113,11 +4116,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>125</v>
       </c>
@@ -4142,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>126</v>
       </c>
@@ -4151,7 +4154,7 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>127</v>
       </c>
@@ -4160,7 +4163,7 @@
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>128</v>
       </c>
@@ -4182,19 +4185,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="117" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="117" workbookViewId="0">
+      <selection activeCell="H147" sqref="H147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="4" width="18" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="12" width="12" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>129</v>
       </c>
@@ -4250,7 +4256,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>43732.333333333001</v>
       </c>
@@ -4284,7 +4290,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>43732.375</v>
       </c>
@@ -4318,7 +4324,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43732.375</v>
       </c>
@@ -4355,7 +4361,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43732.375</v>
       </c>
@@ -4389,7 +4395,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>43732.375</v>
       </c>
@@ -4423,7 +4429,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>43732.375</v>
       </c>
@@ -4457,12 +4463,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>43732.375</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>141</v>
+      </c>
+      <c r="C8">
+        <v>817200436</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -4474,10 +4483,10 @@
         <v>138</v>
       </c>
       <c r="G8" s="6">
-        <v>43732.375</v>
+        <v>43732</v>
       </c>
       <c r="H8" s="6">
-        <v>43732.416666666999</v>
+        <v>43732.041666666664</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -4491,7 +4500,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>43732.375</v>
       </c>
@@ -4525,7 +4534,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>43732.375</v>
       </c>
@@ -4559,7 +4568,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>43732.375</v>
       </c>
@@ -4593,7 +4602,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>43732.375</v>
       </c>
@@ -4627,7 +4636,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>43732.375</v>
       </c>
@@ -4661,7 +4670,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>43732.375</v>
       </c>
@@ -4695,7 +4704,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>43732.375</v>
       </c>
@@ -4729,7 +4738,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4763,7 +4772,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4800,7 +4809,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4834,7 +4843,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4868,7 +4877,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4902,7 +4911,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4936,7 +4945,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4970,7 +4979,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -5004,12 +5013,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>43732.416666666999</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>141</v>
+      </c>
+      <c r="C24">
+        <v>817200436</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
@@ -5021,10 +5033,10 @@
         <v>138</v>
       </c>
       <c r="G24" s="6">
-        <v>43732.416666666999</v>
+        <v>43732.041666666664</v>
       </c>
       <c r="H24" s="6">
-        <v>43732.458333333001</v>
+        <v>43732.083333333336</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -5038,7 +5050,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -5072,7 +5084,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5106,7 +5118,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5140,7 +5152,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5177,7 +5189,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5211,7 +5223,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5245,7 +5257,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5279,7 +5291,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5313,7 +5325,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5347,7 +5359,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5381,7 +5393,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5415,7 +5427,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5449,7 +5461,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5483,7 +5495,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5517,7 +5529,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5551,7 +5563,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5585,7 +5597,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5619,7 +5631,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5653,7 +5665,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5687,7 +5699,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5721,7 +5733,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5755,7 +5767,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5789,7 +5801,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5823,7 +5835,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5857,7 +5869,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>43732.5</v>
       </c>
@@ -5894,7 +5906,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>43732.5</v>
       </c>
@@ -5928,7 +5940,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>43732.5</v>
       </c>
@@ -5962,7 +5974,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>43732.5</v>
       </c>
@@ -5996,7 +6008,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>43732.5</v>
       </c>
@@ -6030,7 +6042,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>43732.5</v>
       </c>
@@ -6064,7 +6076,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>43732.5</v>
       </c>
@@ -6098,7 +6110,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>43732.5</v>
       </c>
@@ -6132,7 +6144,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>43732.5</v>
       </c>
@@ -6166,7 +6178,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>43732.5</v>
       </c>
@@ -6200,7 +6212,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>43732.5</v>
       </c>
@@ -6234,7 +6246,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>43732.5</v>
       </c>
@@ -6268,7 +6280,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>43732.5</v>
       </c>
@@ -6302,7 +6314,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>43732.5</v>
       </c>
@@ -6336,7 +6348,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>43732.5</v>
       </c>
@@ -6370,7 +6382,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>43732.5</v>
       </c>
@@ -6404,7 +6416,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>43732.5</v>
       </c>
@@ -6438,7 +6450,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>43732.5</v>
       </c>
@@ -6472,7 +6484,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6506,7 +6518,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6540,7 +6552,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6574,7 +6586,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6608,7 +6620,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6642,7 +6654,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6676,7 +6688,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6710,7 +6722,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6744,7 +6756,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6778,7 +6790,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6812,7 +6824,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6846,7 +6858,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6880,7 +6892,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6914,7 +6926,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6948,7 +6960,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6982,7 +6994,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7016,7 +7028,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7050,7 +7062,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7084,7 +7096,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7118,7 +7130,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7152,7 +7164,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7186,7 +7198,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7220,7 +7232,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7254,7 +7266,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7288,7 +7300,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7322,7 +7334,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7356,7 +7368,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7390,7 +7402,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7424,7 +7436,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7458,7 +7470,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7492,7 +7504,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7526,7 +7538,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7560,7 +7572,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7594,7 +7606,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7628,7 +7640,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7662,7 +7674,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7696,7 +7708,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7730,7 +7742,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>43732.625</v>
       </c>
@@ -7764,7 +7776,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>43732.625</v>
       </c>
@@ -7798,7 +7810,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>43732.625</v>
       </c>
@@ -7832,7 +7844,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>43732.625</v>
       </c>
@@ -7866,7 +7878,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>43732.625</v>
       </c>
@@ -7900,7 +7912,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>43732.625</v>
       </c>
@@ -7934,7 +7946,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>43732.625</v>
       </c>
@@ -7968,7 +7980,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>43732.625</v>
       </c>
@@ -8002,7 +8014,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>43732.625</v>
       </c>
@@ -8036,7 +8048,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>43732.625</v>
       </c>
@@ -8070,7 +8082,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>43732.625</v>
       </c>
@@ -8104,7 +8116,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>43732.625</v>
       </c>
@@ -8138,7 +8150,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>43732.625</v>
       </c>
@@ -8172,7 +8184,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>43732.625</v>
       </c>
@@ -8206,7 +8218,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>43732.625</v>
       </c>
@@ -8240,7 +8252,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>43732.625</v>
       </c>
@@ -8274,7 +8286,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>43732.625</v>
       </c>
@@ -8308,13 +8320,16 @@
         <v>139</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>43732.666666666999</v>
       </c>
       <c r="B121" t="s">
         <v>140</v>
       </c>
+      <c r="C121">
+        <v>490227758</v>
+      </c>
       <c r="D121" t="s">
         <v>25</v>
       </c>
@@ -8325,10 +8340,10 @@
         <v>138</v>
       </c>
       <c r="G121" s="6">
-        <v>43732.708333333336</v>
+        <v>43732.083333333336</v>
       </c>
       <c r="H121" s="6">
-        <v>43732.75</v>
+        <v>43732.125</v>
       </c>
       <c r="J121">
         <v>1</v>
@@ -8342,7 +8357,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8376,7 +8391,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8410,7 +8425,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8444,7 +8459,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8478,7 +8493,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8512,7 +8527,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8546,7 +8561,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8580,7 +8595,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8614,7 +8629,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8648,7 +8663,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8682,7 +8697,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8716,7 +8731,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8750,7 +8765,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8784,7 +8799,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8818,7 +8833,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8852,7 +8867,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8886,7 +8901,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8920,13 +8935,16 @@
         <v>139</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>43732.708333333001</v>
       </c>
       <c r="B139" t="s">
         <v>140</v>
       </c>
+      <c r="C139">
+        <v>490227758</v>
+      </c>
       <c r="D139" t="s">
         <v>16</v>
       </c>
@@ -8937,10 +8955,10 @@
         <v>138</v>
       </c>
       <c r="G139" s="6">
-        <v>43732.75</v>
+        <v>43732.041666666664</v>
       </c>
       <c r="H139" s="6">
-        <v>43732.791666666664</v>
+        <v>43732.083333333336</v>
       </c>
       <c r="J139">
         <v>1</v>
@@ -8954,7 +8972,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -8988,7 +9006,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9022,7 +9040,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9056,7 +9074,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9090,7 +9108,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9124,7 +9142,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9158,7 +9176,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9192,7 +9210,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9226,7 +9244,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9260,7 +9278,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9294,7 +9312,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9328,7 +9346,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9362,13 +9380,16 @@
         <v>139</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>43732.708333333001</v>
       </c>
       <c r="B152" t="s">
         <v>140</v>
       </c>
+      <c r="C152">
+        <v>490227758</v>
+      </c>
       <c r="D152" t="s">
         <v>67</v>
       </c>
@@ -9379,10 +9400,10 @@
         <v>138</v>
       </c>
       <c r="G152" s="6">
-        <v>0.83333333333333337</v>
+        <v>43732.125</v>
       </c>
       <c r="H152" s="6">
-        <v>0.875</v>
+        <v>43732.166666666664</v>
       </c>
       <c r="J152">
         <v>1</v>
@@ -9396,7 +9417,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="4"/>
       <c r="G153" s="6"/>
       <c r="H153" s="6"/>

</xml_diff>